<commit_message>
Fix development mode - now functional
</commit_message>
<xml_diff>
--- a/YouTube-Comment-Analyzer-Setup.xlsx
+++ b/YouTube-Comment-Analyzer-Setup.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Michelle\Documents\Coding_Projects\Comment-Sentiment-Analyzer\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D80BC479-0EBC-492A-8DF7-E7CE658EA6A0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{22CF461F-C4B4-4648-8ED0-F17538577E52}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -49,7 +49,7 @@
     <t>Step 5: Double-click the file 'run_script_2.bat'</t>
   </si>
   <si>
-    <t>https://www.youtube.com/watch?v=FOqICW5-zgw&amp;ab_channel=TheWildAnimalChannel</t>
+    <t>https://www.youtube.com/watch?v=MDE0outztmc&amp;ab_channel=Curious%3F%3ANaturalWorld</t>
   </si>
 </sst>
 </file>
@@ -119,8 +119,8 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -427,7 +427,7 @@
   <dimension ref="A1:B10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B1" sqref="B1"/>
+      <selection activeCell="A7" sqref="A7:B7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -440,7 +440,7 @@
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="4" t="s">
+      <c r="B1" s="3" t="s">
         <v>9</v>
       </c>
     </row>
@@ -458,34 +458,34 @@
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A6" s="3" t="s">
+      <c r="A6" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="B6" s="3"/>
+      <c r="B6" s="4"/>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A7" s="3" t="s">
+      <c r="A7" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="B7" s="3"/>
+      <c r="B7" s="4"/>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A8" s="3" t="s">
+      <c r="A8" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="B8" s="3"/>
+      <c r="B8" s="4"/>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A9" s="3" t="s">
+      <c r="A9" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="B9" s="3"/>
+      <c r="B9" s="4"/>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A10" s="3" t="s">
+      <c r="A10" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="B10" s="3"/>
+      <c r="B10" s="4"/>
     </row>
   </sheetData>
   <mergeCells count="5">
@@ -495,9 +495,6 @@
     <mergeCell ref="A8:B8"/>
     <mergeCell ref="A6:B6"/>
   </mergeCells>
-  <hyperlinks>
-    <hyperlink ref="B1" r:id="rId1" xr:uid="{6874547C-5DCD-4643-A1A6-39D31D4DCCB4}"/>
-  </hyperlinks>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
 </file>
</xml_diff>